<commit_message>
Set up SQLAlchemy and ingest data.
</commit_message>
<xml_diff>
--- a/app/files/input/Invoices.xlsx
+++ b/app/files/input/Invoices.xlsx
@@ -27,7 +27,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Invoice Qty</t>
+    <t>Invoiced Qty</t>
   </si>
   <si>
     <t>Unit Price</t>
@@ -108,12 +108,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -355,7 +358,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -378,13 +381,13 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>7.0</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>800.0</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <v>5600.0</v>
       </c>
     </row>
@@ -401,13 +404,13 @@
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>15.0</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>15.0</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <v>225.0</v>
       </c>
     </row>
@@ -439,7 +442,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -462,13 +465,13 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>3.0</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>800.0</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <v>2400.0</v>
       </c>
     </row>
@@ -485,13 +488,13 @@
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>12.0</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>25.0</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <v>300.0</v>
       </c>
     </row>
@@ -523,7 +526,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -546,13 +549,13 @@
       <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>6.0</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>150.0</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <v>900.0</v>
       </c>
     </row>
@@ -569,13 +572,13 @@
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>10.0</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>20.0</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <v>200.0</v>
       </c>
     </row>

</xml_diff>